<commit_message>
Added excel with project info
</commit_message>
<xml_diff>
--- a/Kopie - ASEO_4Q2019.xlsx
+++ b/Kopie - ASEO_4Q2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\Screen factory\Projects\official_cdclient\CD\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\Screen factory\Projects\official_cdGitSimon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC5524E-CB23-4396-9312-203C1E5B1C23}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309497E-6C40-4751-9A47-7B348B79CFA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7536" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1035,16 +1035,16 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="4.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>7376</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>7440</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6935</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>7543</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>7541</v>
       </c>
@@ -1177,7 +1177,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>7664</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1217,14 +1217,14 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7495</v>
       </c>
@@ -1242,22 +1242,22 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>7539</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7442</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>7441</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>7542</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>7540</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" t="s">
         <v>40</v>
@@ -1385,16 +1385,16 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.109375" style="3"/>
-    <col min="3" max="3" width="76.5546875" customWidth="1"/>
-    <col min="4" max="4" width="48.44140625" customWidth="1"/>
-    <col min="5" max="5" width="40.5546875" customWidth="1"/>
-    <col min="7" max="7" width="46.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="76.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="7" max="7" width="46.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
@@ -1407,7 +1407,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="4">
         <v>7539</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="255" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>7442</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="270" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>7441</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="4">
         <v>7542</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>7540</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="231" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="231" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>91</v>
       </c>
@@ -1512,25 +1512,25 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" customWidth="1"/>
-    <col min="3" max="6" width="18.44140625" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" customWidth="1"/>
-    <col min="9" max="9" width="73.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>51</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>79</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1689,7 +1689,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>69</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D20" s="12"/>
     </row>
   </sheetData>
@@ -1828,51 +1828,51 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="5.109375" customWidth="1"/>
-    <col min="14" max="20" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" customWidth="1"/>
+    <col min="14" max="20" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N13" s="23" t="s">
         <v>56</v>
       </c>
@@ -1895,37 +1895,37 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
excel - tasks file
</commit_message>
<xml_diff>
--- a/Kopie - ASEO_4Q2019.xlsx
+++ b/Kopie - ASEO_4Q2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\Screen factory\Projects\official_cdGitSimon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9309497E-6C40-4751-9A47-7B348B79CFA5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF92176-5747-4F7F-AC21-1A6B36FF933A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1511,8 +1511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEA2226-BD8B-4145-B6F7-83BF19634D0F}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edit of annex - number of documents removed
</commit_message>
<xml_diff>
--- a/Kopie - ASEO_4Q2019.xlsx
+++ b/Kopie - ASEO_4Q2019.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\Screen factory\Projects\official_cdGitSimon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\Screen factory\simonGit\CDKlient_SimGit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF92176-5747-4F7F-AC21-1A6B36FF933A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6458ADAA-218E-4C59-96E8-2D097D638A52}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>SSE</t>
-  </si>
-  <si>
-    <t>"OPO", "IPO", "TEA", "CW1", "CW2", "CWP", "EUS", "TST"</t>
   </si>
   <si>
     <t>RSS</t>
@@ -483,6 +480,9 @@
   </si>
   <si>
     <t>① chyba s dvěma filtery na enhancement</t>
+  </si>
+  <si>
+    <t>OPO, IPO, TEA, CW1, CW2, CWP, EUS, TST</t>
   </si>
 </sst>
 </file>
@@ -1492,10 +1492,10 @@
     </row>
     <row r="7" spans="2:7" ht="231" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>66</v>
@@ -1512,12 +1512,12 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="6" width="18.42578125" customWidth="1"/>
     <col min="7" max="7" width="34.7109375" customWidth="1"/>
@@ -1535,7 +1535,7 @@
         <v>51</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
@@ -1546,7 +1546,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>45</v>
@@ -1555,14 +1555,14 @@
         <v>50</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>54</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>55</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
@@ -1590,18 +1590,18 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>53</v>
@@ -1611,10 +1611,10 @@
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1637,7 +1637,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
         <v>60</v>
@@ -1796,10 +1796,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>53</v>
@@ -1836,22 +1836,22 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -1859,17 +1859,17 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1892,42 +1892,42 @@
         <v>63</v>
       </c>
       <c r="T13" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C25" s="24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>